<commit_message>
partial DB, registration form, earlier style issues.
Fixing the style issues
base.html
header.html
home.html
ossvol.css

#create the db tables for user and org, and populate skills / language, lang level tables
parts of volunteer_db.sql
dml_preload.sql
models.py

#create the registration form for org / volunteer, does not submit yet, but pulls in existing values for language / skill
ossvol.css
urls.py
views.py
register.html
</commit_message>
<xml_diff>
--- a/progress/Timeline.xlsx
+++ b/progress/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mackosajt\Univeresity\Final_project\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D27C5C-EA0B-488E-A02A-103A7DDF260F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16762107-2047-4BEB-9316-CC96E7D313C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1248" yWindow="684" windowWidth="21048" windowHeight="11532" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Planned</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Completed ahead of time</t>
+  </si>
+  <si>
+    <t>Completed on time</t>
+  </si>
+  <si>
+    <t>Form done, DB insert missing</t>
   </si>
 </sst>
 </file>
@@ -605,7 +611,7 @@
   <dimension ref="A2:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -767,13 +773,19 @@
       <c r="C10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="13"/>
+      <c r="E10" s="3"/>
+      <c r="O10" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="11" spans="1:15">
       <c r="C11" s="12" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="13"/>
+      <c r="O11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:15">
       <c r="C12" s="12" t="s">

</xml_diff>

<commit_message>
Progress report update. Admin page approval in delay
</commit_message>
<xml_diff>
--- a/progress/Timeline.xlsx
+++ b/progress/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mackosajt\Univeresity\Final_project\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16762107-2047-4BEB-9316-CC96E7D313C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E85C266-6524-4D05-89D0-68F5A081C8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1248" yWindow="684" windowWidth="21048" windowHeight="11532" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Planned</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Completed on time</t>
-  </si>
-  <si>
-    <t>Form done, DB insert missing</t>
   </si>
 </sst>
 </file>
@@ -611,7 +608,7 @@
   <dimension ref="A2:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -782,16 +779,16 @@
       <c r="C11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="13"/>
+      <c r="F11" s="3"/>
       <c r="O11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="C12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="13"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:15">
       <c r="C13" s="12" t="s">

</xml_diff>

<commit_message>
admin page for org acceptance
also contains the "not implemented" redirect and progress.
Development is in 1 day delay, this delivery was planned for 06/01/25.
</commit_message>
<xml_diff>
--- a/progress/Timeline.xlsx
+++ b/progress/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mackosajt\Univeresity\Final_project\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E85C266-6524-4D05-89D0-68F5A081C8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2887A3-C28C-45C9-AEB3-E4D05A3D89EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1248" yWindow="684" windowWidth="21048" windowHeight="11532" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Planned</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Completed on time</t>
+  </si>
+  <si>
+    <t>Completed on 07/01/25</t>
   </si>
 </sst>
 </file>
@@ -789,6 +792,9 @@
         <v>14</v>
       </c>
       <c r="F12" s="10"/>
+      <c r="O12" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:15">
       <c r="C13" s="12" t="s">

</xml_diff>

<commit_message>
event create and edit development + bugfixes
</commit_message>
<xml_diff>
--- a/progress/Timeline.xlsx
+++ b/progress/Timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mackosajt\Univeresity\Final_project\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2887A3-C28C-45C9-AEB3-E4D05A3D89EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F182FBCC-E468-4B9C-A233-CC4E43901174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1248" yWindow="684" windowWidth="21048" windowHeight="11532" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -611,7 +612,7 @@
   <dimension ref="A2:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -800,13 +801,13 @@
       <c r="C13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:15">
       <c r="C14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:15">
       <c r="C15" s="12" t="s">

</xml_diff>

<commit_message>
event + apply for event + rest API  demo
#adding single evnet view
#add event application
#add rest api for single event get.
pip install djangorestframework
settings.py
urls.py
api.py
views.py
event.html
events.html
</commit_message>
<xml_diff>
--- a/progress/Timeline.xlsx
+++ b/progress/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mackosajt\Univeresity\Final_project\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F182FBCC-E468-4B9C-A233-CC4E43901174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA20CCE-A49E-4DA8-B2F1-A3BCA3C1BB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1248" yWindow="684" windowWidth="21048" windowHeight="11532" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Planned</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Completed on 07/01/25</t>
+  </si>
+  <si>
+    <t>Enrollment done 14/01/25, not yet acceptance</t>
   </si>
 </sst>
 </file>
@@ -612,7 +615,7 @@
   <dimension ref="A2:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -802,6 +805,9 @@
         <v>15</v>
       </c>
       <c r="G13" s="3"/>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:15">
       <c r="C14" s="12" t="s">

</xml_diff>

<commit_message>
implement pending / approved / rejected volunteers
views.py
event.html
</commit_message>
<xml_diff>
--- a/progress/Timeline.xlsx
+++ b/progress/Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mackosajt\Univeresity\Final_project\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA20CCE-A49E-4DA8-B2F1-A3BCA3C1BB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA0699B-0E3E-4F89-ACD4-43BA2B7DA8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1248" yWindow="684" windowWidth="21048" windowHeight="11532" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18504" windowHeight="11124" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Planned</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Enrollment done 14/01/25, not yet acceptance</t>
+  </si>
+  <si>
+    <t>Completed 17/01/25</t>
   </si>
 </sst>
 </file>
@@ -615,7 +618,7 @@
   <dimension ref="A2:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -814,6 +817,9 @@
         <v>16</v>
       </c>
       <c r="G14" s="10"/>
+      <c r="O14" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="C15" s="12" t="s">

</xml_diff>

<commit_message>
#event recommendation views.py event_recommend.html urls.py events.html # proper event display on HOME and INDEX instead of dummy + fix home button in header. home.html index.html
#event recommendation
views.py
event_recommend.html
urls.py
events.html
# proper event display on HOME and INDEX instead of dummy + fix home button in header.
home.html
index.html
</commit_message>
<xml_diff>
--- a/progress/Timeline.xlsx
+++ b/progress/Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mackosajt\Univeresity\Final_project\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F62A56-3967-4DF9-B13D-D374B9C528C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ADC52A-BF14-4A97-95AA-2CFE938EF6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18504" windowHeight="11124" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Planned</t>
   </si>
@@ -629,7 +629,7 @@
   <dimension ref="A2:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -846,32 +846,38 @@
         <v>18</v>
       </c>
       <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="3:13">
+      <c r="O16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15">
       <c r="C17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="3:13">
+      <c r="I17" s="3"/>
+      <c r="O17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15">
       <c r="C18" s="12" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="3:13">
+    <row r="19" spans="3:15">
       <c r="C19" s="12" t="s">
         <v>21</v>
       </c>
       <c r="K19" s="13"/>
     </row>
-    <row r="20" spans="3:13">
+    <row r="20" spans="3:15">
       <c r="C20" s="12" t="s">
         <v>22</v>
       </c>
       <c r="L20" s="13"/>
     </row>
-    <row r="21" spans="3:13">
+    <row r="21" spans="3:15">
       <c r="C21" s="12" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
unit testing + code validation
11/02/2025
# restricting ZIP input fields
create_edit_event.html
find_event.html

13/02/2025
# add test cases
test.py
# errors out, need specific test user in DB
created UNI_PROJECT_TEST
settings.py # add the test user connect
# still errors out trying to create the user.

14/02/2025
test_runner.py # forcing tester to skip user creation
settings.py # pointing the tester to the skip part

17/02/2025
# cleare schemas from views.py as test.py uses another schema to separate objects
views.py
#add more test cases and fix existing ones.
test.py
</commit_message>
<xml_diff>
--- a/progress/Timeline.xlsx
+++ b/progress/Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mackosajt\Univeresity\Final_project\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55B21AC-8CA8-493B-9AAE-321074E01D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8170F7-1BB2-4CAD-8278-5897ADDEC7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18504" windowHeight="11124" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Planned</t>
   </si>
@@ -131,7 +131,11 @@
   </si>
   <si>
     <t>Server side connection is more complex than expected. 
-03/02/2025 - breaktrhough, chat works, but no restriction yet</t>
+03/02/2025 - breaktrhough, chat works, but no restriction yet
+Complete on 04/02/2025</t>
+  </si>
+  <si>
+    <t>Factory boy complete on 17/02/2025</t>
   </si>
 </sst>
 </file>
@@ -301,6 +305,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,21 +332,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,45 +649,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8857E68D-7487-4353-AE97-7493ACC5C850}">
   <dimension ref="A2:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="2.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="4.88671875" customWidth="1"/>
     <col min="5" max="5" width="5.44140625" customWidth="1"/>
     <col min="6" max="12" width="3.44140625" customWidth="1"/>
     <col min="13" max="13" width="6.109375" customWidth="1"/>
     <col min="14" max="14" width="3.44140625" customWidth="1"/>
-    <col min="15" max="15" width="30.77734375" style="20" customWidth="1"/>
+    <col min="15" max="15" width="30.77734375" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="16" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
       <c r="M2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="22" t="s">
         <v>24</v>
       </c>
     </row>
@@ -721,7 +725,7 @@
       <c r="M3" s="9">
         <v>3</v>
       </c>
-      <c r="O3" s="17"/>
+      <c r="O3" s="22"/>
     </row>
     <row r="4" spans="1:15" ht="15.6">
       <c r="A4" s="10" t="s">
@@ -757,148 +761,151 @@
       <c r="M4" s="11">
         <v>21</v>
       </c>
-      <c r="O4" s="17"/>
+      <c r="O4" s="22"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="14" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="14" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="O9" s="20" t="s">
+      <c r="O9" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="O10" s="20" t="s">
+      <c r="O10" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="10"/>
-      <c r="O12" s="21" t="s">
+      <c r="O12" s="16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="28.8">
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="O13" s="20" t="s">
+      <c r="O13" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="14" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="10"/>
-      <c r="O14" s="21" t="s">
+      <c r="O14" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="28.8">
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="14" t="s">
         <v>17</v>
       </c>
       <c r="H15" s="10"/>
-      <c r="O15" s="22" t="s">
+      <c r="O15" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="14" t="s">
         <v>18</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="O16" s="20" t="s">
+      <c r="O16" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="3:15">
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="O17" s="20" t="s">
+      <c r="O17" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="3:15" ht="57.6">
-      <c r="C18" s="19" t="s">
+    <row r="18" spans="3:15" ht="72">
+      <c r="C18" s="14" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="10"/>
-      <c r="O18" s="20" t="s">
+      <c r="O18" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="3:15">
-      <c r="C19" s="19" t="s">
+    <row r="19" spans="3:15" ht="28.8">
+      <c r="C19" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="12"/>
+      <c r="K19" s="10"/>
+      <c r="O19" s="15" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="3:15">
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="14" t="s">
         <v>22</v>
       </c>
       <c r="L20" s="12"/>
     </row>
     <row r="21" spans="3:15">
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="14" t="s">
         <v>23</v>
       </c>
       <c r="M21" s="12"/>

</xml_diff>

<commit_message>
Finalized timeline + user testing survey results
</commit_message>
<xml_diff>
--- a/progress/Timeline.xlsx
+++ b/progress/Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mackosajt\Univeresity\Final_project\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D52047-5A76-4C3A-870E-6D26D91C23DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7C718A-F4D6-4B91-8D63-333163DA13CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1188" yWindow="2700" windowWidth="18024" windowHeight="9324" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
+    <workbookView xWindow="1920" yWindow="348" windowWidth="18420" windowHeight="11988" xr2:uid="{AFE011C7-FFB9-41D4-BA25-ABE59DD8CB1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Planned</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Factory boy complete on 17/02/2025</t>
+  </si>
+  <si>
+    <t>Last reply complete on 13/03/2025</t>
+  </si>
+  <si>
+    <t>No bugfix request from users, other fixes were implemented earlier.</t>
   </si>
 </sst>
 </file>
@@ -206,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,12 +267,6 @@
         <bgColor rgb="FFD8D8D8"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor rgb="FF6FA8DC"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -280,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,7 +315,6 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -344,7 +343,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,45 +659,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8857E68D-7487-4353-AE97-7493ACC5C850}">
   <dimension ref="A2:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="2.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="12" customWidth="1"/>
     <col min="4" max="4" width="4.88671875" customWidth="1"/>
     <col min="5" max="5" width="5.44140625" customWidth="1"/>
     <col min="6" max="12" width="3.44140625" customWidth="1"/>
     <col min="13" max="13" width="6.109375" customWidth="1"/>
     <col min="14" max="14" width="3.44140625" customWidth="1"/>
-    <col min="15" max="15" width="30.77734375" style="15" customWidth="1"/>
+    <col min="15" max="15" width="38.44140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="18"/>
+      <c r="F2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="21" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
       <c r="M2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="21" t="s">
         <v>24</v>
       </c>
     </row>
@@ -737,7 +735,7 @@
       <c r="M3" s="9">
         <v>3</v>
       </c>
-      <c r="O3" s="22"/>
+      <c r="O3" s="21"/>
     </row>
     <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -773,154 +771,160 @@
       <c r="M4" s="11">
         <v>21</v>
       </c>
-      <c r="O4" s="22"/>
+      <c r="O4" s="21"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="O9" s="15" t="s">
+      <c r="O9" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="O10" s="15" t="s">
+      <c r="O10" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="10"/>
-      <c r="O12" s="16" t="s">
+      <c r="O12" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="3"/>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="10"/>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>17</v>
       </c>
       <c r="H15" s="10"/>
-      <c r="O15" s="17" t="s">
+      <c r="O15" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>19</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="O17" s="15" t="s">
+      <c r="O17" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="3:15" ht="72" x14ac:dyDescent="0.3">
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="10"/>
-      <c r="O18" s="15" t="s">
+      <c r="O18" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="3:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C19" s="14" t="s">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C19" s="13" t="s">
         <v>21</v>
       </c>
       <c r="K19" s="10"/>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L20" s="23"/>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
-      <c r="C21" s="14" t="s">
+      <c r="L20" s="10"/>
+      <c r="O20" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C21" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M21" s="12"/>
+      <c r="M21" s="10"/>
+      <c r="O21" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>